<commit_message>
renaming DatabaseRefernce-->Identifier; ignoring WPS temp files
</commit_message>
<xml_diff>
--- a/tests/fixtures/migrate/example-wc_lang-model.xlsx
+++ b/tests/fixtures/migrate/example-wc_lang-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="993" firstSheet="8" activeTab="21"/>
+    <workbookView windowWidth="20295" windowHeight="6840" tabRatio="993" firstSheet="12" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
     <t>second</t>
   </si>
   <si>
-    <t>Database references</t>
+    <t>Identifiers</t>
   </si>
   <si>
     <t>Comments</t>
@@ -6557,10 +6557,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -6594,53 +6594,13 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6660,8 +6620,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6682,16 +6675,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6705,6 +6719,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -6712,31 +6734,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6757,13 +6757,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6775,19 +6793,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6799,31 +6805,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6835,31 +6817,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6877,7 +6841,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6889,49 +6931,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6951,21 +6951,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -6975,17 +6960,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -7001,17 +6982,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -7034,8 +7004,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -7043,144 +7013,174 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -19927,12 +19927,12 @@
   <sheetPr/>
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
@@ -19992,7 +19992,7 @@
   <sheetPr/>
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>

</xml_diff>

<commit_message>
updating for changes to wc-onto
</commit_message>
<xml_diff>
--- a/tests/fixtures/migrate/example-wc_lang-model.xlsx
+++ b/tests/fixtures/migrate/example-wc_lang-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="6840" tabRatio="993" firstSheet="12" activeTab="20"/>
+    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="993" firstSheet="12" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -5963,7 +5963,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>experimental_evidence</t>
+    <t>experimental_observation</t>
   </si>
   <si>
     <t>Mycoplasma genitalium</t>
@@ -6008,7 +6008,7 @@
     <t>evidence 002</t>
   </si>
   <si>
-    <t>computational_evidence</t>
+    <t>computational_observation</t>
   </si>
   <si>
     <t>Mycoplasma pneumoniae</t>
@@ -6017,7 +6017,7 @@
     <t>Evidence 003</t>
   </si>
   <si>
-    <t>theoretical_evidence</t>
+    <t>theoretical_observation</t>
   </si>
   <si>
     <t>Escherichia coli</t>
@@ -6594,20 +6594,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6621,40 +6610,27 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6669,7 +6645,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6682,15 +6666,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6704,39 +6720,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6757,91 +6757,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6853,7 +6769,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6871,7 +6793,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6883,7 +6859,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6895,7 +6871,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6907,37 +6913,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6962,11 +6962,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -7001,24 +6999,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -7030,6 +7010,17 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -7048,139 +7039,148 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -18587,12 +18587,12 @@
   <sheetPr/>
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -18877,7 +18877,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -19927,7 +19927,7 @@
   <sheetPr/>
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>

</xml_diff>